<commit_message>
feat: finish chineseyi_related function
</commit_message>
<xml_diff>
--- a/chineseyi.xlsx
+++ b/chineseyi.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,22 +430,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>星期</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>上/下午</t>
-        </is>
-      </c>
-      <c r="D1" t="inlineStr">
-        <is>
-          <t>時間</t>
-        </is>
-      </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>老師</t>
+          <t>(時間,老師,年級)</t>
         </is>
       </c>
     </row>
@@ -457,22 +442,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>3-5</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>黃怡萍</t>
+          <t>[('3-5', '黃怡萍', '四')]</t>
         </is>
       </c>
     </row>
@@ -484,17 +454,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
@@ -506,17 +466,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
@@ -528,49 +478,19 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>吳汐淇</t>
+          <t>[('3-4', '吳汐淇', '四'), ('4-5', '柯道維', '四')]</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>113/09/30</t>
+          <t>113/10/07</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>4-5</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>柯道維</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -582,17 +502,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
@@ -604,17 +514,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
@@ -626,22 +526,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3-5</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>張凱博</t>
+          <t>[('3-5', '張凱博', '四')]</t>
         </is>
       </c>
     </row>
@@ -653,282 +538,115 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>林詩怡</t>
+          <t>[('3-4', '林詩怡', '四'), ('4-5', '林詩怡', '四')]</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>113/11/04</t>
+          <t>113/11/11</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>4-5</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>林詩怡</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>113/11/11</t>
+          <t>113/11/18</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', None, '四')]</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>113/11/18</t>
+          <t>113/11/25</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>3-5</t>
+          <t>[('3-5', '賴弘岳', '四')]</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>113/11/25</t>
+          <t>113/12/02</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>3-5</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>賴弘岳</t>
+          <t>[('3-4', '王子源', '四'), ('4-5', '曾睿玉', '四')]</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>113/12/02</t>
+          <t>113/12/09</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>王子源</t>
+          <t>[('3-4', '黃志平', '四'), ('4-5', '黃志平', '四')]</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>113/12/02</t>
+          <t>113/12/16</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>4-5</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>曾睿玉</t>
+          <t>[('3-4', '賴弘岳', '四')]</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>113/12/09</t>
+          <t>113/12/23</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>黃志平</t>
+          <t>[('3-4', '劉良智', '四')]</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>113/12/09</t>
+          <t>113/12/30</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>4-5</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>黃志平</t>
+          <t>[]</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>113/12/16</t>
+          <t>114/01/06</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>賴弘岳</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>113/12/23</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>一)</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>P</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>3-4</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>劉良智</t>
+          <t>[]</t>
         </is>
       </c>
     </row>

</xml_diff>